<commit_message>
Localization Updates, Clementine moved to Tier 7, Basic Redstone and Vanguard parts moved to Tier 1, and Klaws rebalanced into the robotics tree
</commit_message>
<xml_diff>
--- a/Versioning/ModSupportAnalysis.xlsx
+++ b/Versioning/ModSupportAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Kerbal Space Program\GameData\SkyhawkScienceSystem\Versioning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC122DAB-34C4-42B4-A071-7E1BE537506B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECB8FD2-7004-4EAC-BC3E-2B38B30AF9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6708" yWindow="4224" windowWidth="15228" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,19 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={65900EE2-EFD1-44D1-A665-A81EE3D61A26}</author>
     <author>tc={BAD45277-6BB8-474E-812D-834F260C303D}</author>
   </authors>
   <commentList>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{BAD45277-6BB8-474E-812D-834F260C303D}">
+    <comment ref="B35" authorId="0" shapeId="0" xr:uid="{65900EE2-EFD1-44D1-A665-A81EE3D61A26}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Never touched BG science...</t>
+      </text>
+    </comment>
+    <comment ref="B44" authorId="1" shapeId="0" xr:uid="{BAD45277-6BB8-474E-812D-834F260C303D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -43,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="98">
   <si>
     <t>Mod Name</t>
   </si>
@@ -63,9 +72,6 @@
     <t>Hard Requirement - Must be installed for SSS to properly function (Ex. Community Resource Pack)</t>
   </si>
   <si>
-    <t>Soft Requirement - Aren't truly required for SSS to function properly, but are heavily recommended for the full experience (Ex. Rational Resources)</t>
-  </si>
-  <si>
     <t>Supported - Parts are given SSS tech placements, and basic patches (hypergolic engines and tankswitches) are applied, but other things, such as custom science experiments or custom mechanics are not (Ex. Tarsier Space Telescopes)</t>
   </si>
   <si>
@@ -115,13 +121,238 @@
   </si>
   <si>
     <t>Science Param Editor</t>
+  </si>
+  <si>
+    <t>Restock</t>
+  </si>
+  <si>
+    <t>Restock+</t>
+  </si>
+  <si>
+    <t>reDIRECT</t>
+  </si>
+  <si>
+    <t>PhotonCorp</t>
+  </si>
+  <si>
+    <t>Hephaistos</t>
+  </si>
+  <si>
+    <t>Tundra Exploration</t>
+  </si>
+  <si>
+    <t>Tundra Technologies</t>
+  </si>
+  <si>
+    <t>Cryogenic Engines</t>
+  </si>
+  <si>
+    <t>Kerbal Atomics</t>
+  </si>
+  <si>
+    <t>Far Future Technologies</t>
+  </si>
+  <si>
+    <t>Missing History</t>
+  </si>
+  <si>
+    <t>Near Future Launch Vehicles</t>
+  </si>
+  <si>
+    <t>Near Future Propulsion</t>
+  </si>
+  <si>
+    <t>Rocket Motor Menagerie</t>
+  </si>
+  <si>
+    <t>Coatl Aerospace/Probes Plus</t>
+  </si>
+  <si>
+    <t>Heat Control</t>
+  </si>
+  <si>
+    <t>Stockalike Station Parts Redux</t>
+  </si>
+  <si>
+    <t>Kerbal Planetary Base Systems</t>
+  </si>
+  <si>
+    <t>Near Future Electrics</t>
+  </si>
+  <si>
+    <t>Near Future Exploration</t>
+  </si>
+  <si>
+    <t>Near Future Solar</t>
+  </si>
+  <si>
+    <t>Near Future Construction</t>
+  </si>
+  <si>
+    <t>Near Future Spacecraft</t>
+  </si>
+  <si>
+    <t>Completely Non-Aggressive Rocketry</t>
+  </si>
+  <si>
+    <t>Special Delivery</t>
+  </si>
+  <si>
+    <t>Boring Crew Services</t>
+  </si>
+  <si>
+    <t>Airplane Plus</t>
+  </si>
+  <si>
+    <t>Shuttle Orbiter Construction Kit</t>
+  </si>
+  <si>
+    <t>Mk2 Expansion</t>
+  </si>
+  <si>
+    <t>Mk3 Expansion</t>
+  </si>
+  <si>
+    <t>Near Future Aeronautics</t>
+  </si>
+  <si>
+    <t>Mark IV Spaceplane System</t>
+  </si>
+  <si>
+    <t>Chrayol Design Org</t>
+  </si>
+  <si>
+    <t>Commonwealth Rocketry Establishment</t>
+  </si>
+  <si>
+    <t>Blue Steel/Commonwealth Aeronautics</t>
+  </si>
+  <si>
+    <t>Provenance Aerospace</t>
+  </si>
+  <si>
+    <t>Luciole</t>
+  </si>
+  <si>
+    <t>Ziegler Launch System</t>
+  </si>
+  <si>
+    <t>GemstoneLV</t>
+  </si>
+  <si>
+    <t>Dodo Labs</t>
+  </si>
+  <si>
+    <t>Kerwis Chinese Aerospace Pack</t>
+  </si>
+  <si>
+    <t>Kertemis Program</t>
+  </si>
+  <si>
+    <t>Konstellation Program</t>
+  </si>
+  <si>
+    <t>X-20 Moroz</t>
+  </si>
+  <si>
+    <t>MK-33</t>
+  </si>
+  <si>
+    <t>Fuji Capsule</t>
+  </si>
+  <si>
+    <t>Shangsheng Orbital</t>
+  </si>
+  <si>
+    <t>DSSHU</t>
+  </si>
+  <si>
+    <t>BonVoyage</t>
+  </si>
+  <si>
+    <t>CommNetAntennasExtension</t>
+  </si>
+  <si>
+    <t>ConformalDecals</t>
+  </si>
+  <si>
+    <t>DeepFreeze</t>
+  </si>
+  <si>
+    <t>Kerbal Attachment System</t>
+  </si>
+  <si>
+    <t>Kerbal Inventory System</t>
+  </si>
+  <si>
+    <t>KeR-7</t>
+  </si>
+  <si>
+    <t>Kerbal Engineer</t>
+  </si>
+  <si>
+    <t>Planetside Exploration Technologies</t>
+  </si>
+  <si>
+    <t>HabTech2</t>
+  </si>
+  <si>
+    <t>RemoteTechRedev</t>
+  </si>
+  <si>
+    <t>UniversalStorage2</t>
+  </si>
+  <si>
+    <t>Kerbal GPS Revived</t>
+  </si>
+  <si>
+    <t>MK-1 Stockalike Open Cockpit</t>
+  </si>
+  <si>
+    <t>Missing Robotics</t>
+  </si>
+  <si>
+    <t>Stockish Project Orion</t>
+  </si>
+  <si>
+    <t>kOS</t>
+  </si>
+  <si>
+    <t>Stockalike Mining Expansion</t>
+  </si>
+  <si>
+    <t>Rational Resources Parts</t>
+  </si>
+  <si>
+    <t>Rational Resources Nuclear Family</t>
+  </si>
+  <si>
+    <t>MechJeb</t>
+  </si>
+  <si>
+    <t>Tea Kettle RCS</t>
+  </si>
+  <si>
+    <t>Kerbal Reusability Expansion</t>
+  </si>
+  <si>
+    <t>Soft Requirement - Aren't truly required for SSS to function properly, but are required for certain features to work, such as fuel cell and ntr switches (Ex. Rational Resources)</t>
+  </si>
+  <si>
+    <t>Supported*/Integrated* - Mods within their respective tiers which I highly recommend considering for your playthrough, as they help to fill out empty parts of the tree, and otherwise are very enjoyable to play</t>
+  </si>
+  <si>
+    <t>Integrated*</t>
+  </si>
+  <si>
+    <t>Supported*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +366,12 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -144,7 +381,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -191,15 +428,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,7 +758,10 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B11" dT="2021-12-02T22:29:42.45" personId="{D7652A53-5586-48BB-862A-593C2B58CA62}" id="{BAD45277-6BB8-474E-812D-834F260C303D}">
+  <threadedComment ref="B35" dT="2021-12-02T22:29:42.45" personId="{D7652A53-5586-48BB-862A-593C2B58CA62}" id="{65900EE2-EFD1-44D1-A665-A81EE3D61A26}">
+    <text>Never touched BG science...</text>
+  </threadedComment>
+  <threadedComment ref="B44" dT="2021-12-02T22:29:42.45" personId="{D7652A53-5586-48BB-862A-593C2B58CA62}" id="{BAD45277-6BB8-474E-812D-834F260C303D}">
     <text>Never touched BG science...</text>
   </threadedComment>
 </ThreadedComments>
@@ -494,15 +769,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D6" sqref="D2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="38.88671875" customWidth="1"/>
     <col min="2" max="3" width="17.6640625" customWidth="1"/>
     <col min="4" max="4" width="171.33203125" customWidth="1"/>
   </cols>
@@ -520,10 +795,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
@@ -531,106 +806,681 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
+      <c r="A11" s="9" t="s">
+        <v>90</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
+      <c r="A12" s="9" t="s">
+        <v>89</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="A13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B84" s="8"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B85" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B13">
-    <sortCondition ref="B2:B13"/>
-    <sortCondition ref="A2:A13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B83">
+    <sortCondition ref="B2:B83" customList="This is the Mod,Hard Requirement,Soft Requirement,Integrated*,Integrated,Supported*,Supported"/>
+    <sortCondition ref="A2:A83"/>
   </sortState>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>